<commit_message>
Modified login,registration,forgotpassword and trackorderpage testcases and Implemented log4j
</commit_message>
<xml_diff>
--- a/src/resources/testdata/loginTestdata.xlsx
+++ b/src/resources/testdata/loginTestdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivam_kushwaha\eclipse-workspace\ShoppingPortal\src\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D49E993-0402-4298-9D70-8E7C03128421}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888C9B2B-5DF8-4784-BC47-C5759A240217}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AB54F580-19EE-47DC-8C69-0A67E8BEB4B3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{7890D6BD-CEB1-40C7-AF39-640BB0C26A11}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Positive Testdata" sheetId="1" r:id="rId1"/>
+    <sheet name="Negative Testdata" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,39 +35,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
-  <si>
-    <t>password</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
   <si>
     <t>sk@g.com</t>
   </si>
   <si>
+    <t>sk@12345</t>
+  </si>
+  <si>
+    <t>ok@g.com</t>
+  </si>
+  <si>
+    <t>ok@12345</t>
+  </si>
+  <si>
+    <t>pk@g.com</t>
+  </si>
+  <si>
+    <t>pk@12345</t>
+  </si>
+  <si>
+    <t>fake9@g.com</t>
+  </si>
+  <si>
+    <t>fake@12345</t>
+  </si>
+  <si>
     <t>abc@f.com</t>
   </si>
   <si>
+    <t>abc#123</t>
+  </si>
+  <si>
     <t>def@g.com</t>
   </si>
   <si>
+    <t>df@456</t>
+  </si>
+  <si>
     <t>ghi@g.com</t>
   </si>
   <si>
-    <t>email</t>
+    <t>jk789</t>
   </si>
   <si>
     <t>hjk@g.com</t>
   </si>
   <si>
-    <t>sk@12345</t>
-  </si>
-  <si>
-    <t>fail</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expected </t>
+    <t>we@123</t>
   </si>
 </sst>
 </file>
@@ -82,17 +104,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -123,15 +145,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -446,104 +465,146 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACC2C49-9A3E-4824-AAE4-18F3C9C2FB25}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC91A5C6-7C17-47CE-8C29-E81EC195F79F}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.6328125" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>123</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>456</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>789</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>123</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" xr:uid="{75840057-C67A-41F8-B8A3-32FA4AA6DBFF}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{A5A1AE59-4484-4C12-B00B-334D7E29191C}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{E6C7C7D3-CF5A-4989-9479-5D3A2569610A}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{E1687DFC-0A1C-4D3A-9E66-6D0C70954948}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{DC3EFE44-E790-4841-BD60-7301CD12EEEF}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{D224B78F-C5F6-4C04-8CF0-3F0FEBF6EB2D}"/>
-    <hyperlink ref="A7" r:id="rId7" xr:uid="{047D08DA-2256-44A7-8ECE-C81785E79D93}"/>
-    <hyperlink ref="B7" r:id="rId8" xr:uid="{E2867F5D-4033-4A68-8077-BEEB64C4946A}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{423F372F-CB28-407A-B501-A831CCD5550A}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{35E493D1-5E42-4AC0-9DA8-F93C00F1C45A}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{CA8B18FF-2567-4195-85F3-23C42DD6BE02}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{D2740599-B669-4310-8B28-04F6A0861ECF}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{2F26A720-94BF-4E90-B241-53725762E769}"/>
+    <hyperlink ref="A5" r:id="rId6" xr:uid="{5059981D-4638-4F1D-86CF-F0FB36EE6443}"/>
+    <hyperlink ref="B5" r:id="rId7" xr:uid="{5BA55FBB-FC54-4CA0-B130-4802A6824B08}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47CCCB2-40D9-4DD9-8176-CF279C3F80CE}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.6328125" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" xr:uid="{D7F6D9EF-CEA5-40AD-8ACD-F5C3CC6E3AFC}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{CEEE1DCF-9DFD-4B34-B2D7-8523CFEF5136}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{E558B136-671E-4BD3-88F3-345FF5D0BA1B}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{120149B6-1DC3-4822-B8E4-D10303C4973D}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{E8E1612C-B858-4D09-955F-52C7670D8976}"/>
+    <hyperlink ref="A6" r:id="rId6" xr:uid="{D64E2D72-E1AF-4672-9226-4A5A75E59587}"/>
+    <hyperlink ref="B3" r:id="rId7" xr:uid="{F59A3FF9-4003-4305-BD87-CFF3ADBD7B16}"/>
+    <hyperlink ref="B6" r:id="rId8" xr:uid="{E0D477D7-E8E5-425F-8487-E5109363C01F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>